<commit_message>
PM und Design Bilder
</commit_message>
<xml_diff>
--- a/Projekt Management/Zeiterfassung.xlsx
+++ b/Projekt Management/Zeiterfassung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://htldornbirn-my.sharepoint.com/personal/linus_woerndle_student_htldornbirn_at/Documents/4. Jahr/Softwareentwicklung und Projektmanagement/5. AA - Projekt - HomeSphere/HomeSphere/Projekt Management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="498" documentId="13_ncr:1_{B0761948-1EC6-46FA-9F5A-F6DD0D3AA1F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B843F0B-6CFA-4CE4-9423-45C84FE94349}"/>
+  <xr:revisionPtr revIDLastSave="503" documentId="13_ncr:1_{B0761948-1EC6-46FA-9F5A-F6DD0D3AA1F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D14DCC68-EA2E-40FC-9831-7097DC9CAE41}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{8CF7A9F1-50C4-41E0-98B0-08DA5C94E484}"/>
   </bookViews>
@@ -1890,15 +1890,15 @@
       </c>
       <c r="K3" s="18" t="str">
         <f>INT(SUBSTITUTE(SUM(C3:C1048576),"min","")/60)&amp;" h "&amp;MOD(SUBSTITUTE(SUM(C3:C1048576),"min",""),60)&amp;" min"</f>
-        <v>4 h 20 min</v>
+        <v>5 h 0 min</v>
       </c>
       <c r="L3" s="149" t="str">
         <f>INT(SUBSTITUTE(SUM(D3:D1048576),"min","")/60)&amp;" h "&amp;MOD(SUBSTITUTE(SUM(D3:D1048576),"min",""),60)&amp;" min"</f>
-        <v>3 h 50 min</v>
+        <v>4 h 30 min</v>
       </c>
       <c r="M3" s="150" t="str">
         <f>INT(SUBSTITUTE(SUM(E3:E1048576),"min","")/60)&amp;" h "&amp;MOD(SUBSTITUTE(SUM(E3:E1048576),"min",""),60)&amp;" min"</f>
-        <v>4 h 30 min</v>
+        <v>4 h 40 min</v>
       </c>
       <c r="N3" s="12" t="str">
         <f>INT(SUBSTITUTE(SUM(F3:F1048576),"min","")/60)&amp;" h "&amp;MOD(SUBSTITUTE(SUM(F3:F1048576),"min",""),60)&amp;" min"</f>
@@ -2013,7 +2013,7 @@
         <v>142</v>
       </c>
       <c r="C12">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>12</v>
@@ -2026,8 +2026,11 @@
       <c r="B13" s="2" t="s">
         <v>143</v>
       </c>
+      <c r="C13">
+        <v>65</v>
+      </c>
       <c r="D13">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="I13" s="20">
         <v>45477</v>
@@ -2041,7 +2044,7 @@
         <v>144</v>
       </c>
       <c r="E14">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>